<commit_message>
feat: aplica regras de negócio na base tratada
</commit_message>
<xml_diff>
--- a/data/processed/visitas_matricula_tratadas.xlsx
+++ b/data/processed/visitas_matricula_tratadas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29711"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B4D12CB-CB35-4E4D-BA48-ADC0559D1B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC1DECF2-2995-4403-B5D6-C41BE854068D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>id_visita</t>
   </si>
@@ -103,7 +103,16 @@
     <t>Mariana Alves</t>
   </si>
   <si>
-    <t>visita_realizada_flag</t>
+    <t>visita_valida</t>
+  </si>
+  <si>
+    <t>status_normalizado</t>
+  </si>
+  <si>
+    <t>fluxo</t>
+  </si>
+  <si>
+    <t>flag_instalacao_hidrometro</t>
   </si>
 </sst>
 </file>
@@ -139,8 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -459,7 +471,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E6" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -497,7 +509,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>46024</v>
       </c>
       <c r="C2" t="s">
@@ -523,7 +535,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>46024</v>
       </c>
       <c r="C3" t="s">
@@ -540,7 +552,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>46025</v>
       </c>
       <c r="C4" t="s">
@@ -557,7 +569,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>46025</v>
       </c>
       <c r="C5" t="s">
@@ -583,7 +595,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>46026</v>
       </c>
       <c r="C6" t="s">
@@ -612,21 +624,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8BDE71-58D6-409F-B2FB-5928BCF34052}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I2" sqref="I2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,10 +659,186 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30.75">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>46024</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>IF(OR(E2="",E2="ERRO"),"Não","Sim")</f>
+        <v>Sim</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(E2="SUCESSO","CAPTADO",
+IF(E2="AUSENTE","AUSENTE",
+IF(E2="RECUSA","RECUSA","OUTRO")))</f>
+        <v>CAPTADO</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(G2="CAPTADO","segue_para_capex","encerrado_na_visita")</f>
+        <v>segue_para_capex</v>
+      </c>
+      <c r="I2" t="str">
+        <f>IF(H2="segue_para_capex","Sim","Não")</f>
+        <v>Sim</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>46024</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>IF(OR(E3="",E3="ERRO"),"Não","Sim")</f>
+        <v>Sim</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G6" si="0">IF(E3="SUCESSO","CAPTADO",
+IF(E3="AUSENTE","AUSENTE",
+IF(E3="RECUSA","RECUSA","OUTRO")))</f>
+        <v>AUSENTE</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H6" si="1">IF(G3="CAPTADO","segue_para_capex","encerrado_na_visita")</f>
+        <v>encerrado_na_visita</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I6" si="2">IF(H3="segue_para_capex","Sim","Não")</f>
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>46025</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" ref="F3:F6" si="3">IF(OR(E4="",E4="ERRO"),"Não","Sim")</f>
+        <v>Sim</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>RECUSA</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>encerrado_na_visita</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="2"/>
+        <v>Não</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>46025</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Sim</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>CAPTADO</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>segue_para_capex</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="2"/>
+        <v>Sim</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>23</v>
+      <c r="B6" s="2">
+        <v>46026</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Sim</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>CAPTADO</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>segue_para_capex</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="2"/>
+        <v>Sim</v>
       </c>
     </row>
   </sheetData>

</xml_diff>